<commit_message>
added monthly and yearly outcome_ath dictionaries
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\fetal\forGithub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BC60EE-5F57-433E-BD07-38215BA344FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F8BC60EE-5F57-433E-BD07-38215BA344FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F0BE015-B8B1-404B-ACE2-704CB8F8A95C}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="2" r:id="rId1"/>
     <sheet name="Categories" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -69,10 +82,16 @@
     <t>label</t>
   </si>
   <si>
-    <t>alias</t>
-  </si>
-  <si>
-    <t>variable</t>
+    <t>row_id</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Unique identifer for the row in Opal</t>
   </si>
   <si>
     <t>mother_id</t>
@@ -90,100 +109,19 @@
     <t xml:space="preserve">Unique identifier number for the index child </t>
   </si>
   <si>
+    <t>cohort_id</t>
+  </si>
+  <si>
+    <t>Unique identifier for the cohort</t>
+  </si>
+  <si>
     <t>CRL_t1</t>
   </si>
   <si>
+    <t>decimal</t>
+  </si>
+  <si>
     <t>cm</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>cohort_id</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>sws</t>
-  </si>
-  <si>
-    <t>alspac</t>
-  </si>
-  <si>
-    <t>dnbc</t>
-  </si>
-  <si>
-    <t>bib</t>
-  </si>
-  <si>
-    <t>gecko</t>
-  </si>
-  <si>
-    <t>rhea</t>
-  </si>
-  <si>
-    <t>moba</t>
-  </si>
-  <si>
-    <t>elfe</t>
-  </si>
-  <si>
-    <t>eden</t>
-  </si>
-  <si>
-    <t>nfbc66</t>
-  </si>
-  <si>
-    <t>nfbc86</t>
-  </si>
-  <si>
-    <t>hbcs</t>
-  </si>
-  <si>
-    <t>chop</t>
-  </si>
-  <si>
-    <t>raine</t>
-  </si>
-  <si>
-    <t>rug</t>
-  </si>
-  <si>
-    <t>kanc</t>
-  </si>
-  <si>
-    <t>gaspii</t>
-  </si>
-  <si>
-    <t>piccolipu</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>bisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">environage </t>
-  </si>
-  <si>
-    <t>pelagie</t>
-  </si>
-  <si>
-    <t>sepages</t>
-  </si>
-  <si>
-    <t>tng</t>
-  </si>
-  <si>
-    <t>hgs</t>
-  </si>
-  <si>
-    <t>recetox</t>
-  </si>
-  <si>
-    <t>genxxi</t>
   </si>
   <si>
     <r>
@@ -208,16 +146,10 @@
     </r>
   </si>
   <si>
-    <t>row_id</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>Unique identifer for the row in Opal</t>
-  </si>
-  <si>
-    <t>Unique identifier for the cohort</t>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>isMissing</t>
   </si>
   <si>
     <t>genr</t>
@@ -229,17 +161,95 @@
     <t>ninfea</t>
   </si>
   <si>
-    <t>isMissing</t>
+    <t>sws</t>
+  </si>
+  <si>
+    <t>alspac</t>
+  </si>
+  <si>
+    <t>dnbc</t>
+  </si>
+  <si>
+    <t>bib</t>
+  </si>
+  <si>
+    <t>gecko</t>
+  </si>
+  <si>
+    <t>rhea</t>
+  </si>
+  <si>
+    <t>moba</t>
+  </si>
+  <si>
+    <t>elfe</t>
+  </si>
+  <si>
+    <t>eden</t>
+  </si>
+  <si>
+    <t>nfbc66</t>
+  </si>
+  <si>
+    <t>nfbc86</t>
+  </si>
+  <si>
+    <t>hbcs</t>
+  </si>
+  <si>
+    <t>chop</t>
+  </si>
+  <si>
+    <t>raine</t>
+  </si>
+  <si>
+    <t>rug</t>
+  </si>
+  <si>
+    <t>kanc</t>
+  </si>
+  <si>
+    <t>gaspii</t>
+  </si>
+  <si>
+    <t>piccolipu</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>bisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environage </t>
   </si>
   <si>
     <t>no_name</t>
+  </si>
+  <si>
+    <t>pelagie</t>
+  </si>
+  <si>
+    <t>sepages</t>
+  </si>
+  <si>
+    <t>tng</t>
+  </si>
+  <si>
+    <t>hgs</t>
+  </si>
+  <si>
+    <t>recetox</t>
+  </si>
+  <si>
+    <t>genxxi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -353,12 +363,6 @@
     <font>
       <sz val="11"/>
       <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -391,27 +395,8 @@
       <name val="Arial"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="20">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,18 +497,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="27"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -672,30 +645,14 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1204,96 +1161,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1313,513 +1264,465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>104</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>105</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>107</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>108</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>109</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>111</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>112</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>113</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>114</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>115</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>116</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>117</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>118</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>119</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>120</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>121</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>122</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>123</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>124</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>125</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>126</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>127</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>128</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>129</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>131</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6">
-        <v>101</v>
-      </c>
-      <c r="C2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6">
-        <v>102</v>
-      </c>
-      <c r="C3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6">
-        <v>103</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="6">
-        <v>104</v>
-      </c>
-      <c r="C5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6">
-        <v>105</v>
-      </c>
-      <c r="C6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6">
-        <v>106</v>
-      </c>
-      <c r="C7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="6">
-        <v>107</v>
-      </c>
-      <c r="C8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="6">
-        <v>108</v>
-      </c>
-      <c r="C9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="6">
-        <v>109</v>
-      </c>
-      <c r="C10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6">
-        <v>110</v>
-      </c>
-      <c r="C11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6">
-        <v>111</v>
-      </c>
-      <c r="C12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6">
-        <v>112</v>
-      </c>
-      <c r="C13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6">
-        <v>113</v>
-      </c>
-      <c r="C14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6">
-        <v>114</v>
-      </c>
-      <c r="C15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6">
-        <v>115</v>
-      </c>
-      <c r="C16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6">
-        <v>116</v>
-      </c>
-      <c r="C17" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="6">
-        <v>117</v>
-      </c>
-      <c r="C18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6">
-        <v>118</v>
-      </c>
-      <c r="C19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="7">
-        <v>119</v>
-      </c>
-      <c r="C20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="6">
-        <v>120</v>
-      </c>
-      <c r="C21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="6">
-        <v>121</v>
-      </c>
-      <c r="C22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="6">
-        <v>122</v>
-      </c>
-      <c r="C23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="6">
-        <v>123</v>
-      </c>
-      <c r="C24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="6">
-        <v>124</v>
-      </c>
-      <c r="C25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="7">
-        <v>125</v>
-      </c>
-      <c r="C26" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="6">
-        <v>126</v>
-      </c>
-      <c r="C27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="6">
-        <v>127</v>
-      </c>
-      <c r="C28" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="6">
-        <v>128</v>
-      </c>
-      <c r="C29" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="6">
-        <v>129</v>
-      </c>
-      <c r="C30" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="6">
-        <v>130</v>
-      </c>
-      <c r="C31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="6">
-        <v>131</v>
-      </c>
-      <c r="C32" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
fix outcome_ath non_rep and yearly_rep xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\fetal\forGithub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\extender_outcomes_ath\20230321_outcomes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F8BC60EE-5F57-433E-BD07-38215BA344FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB8DD2D0-A5A4-4CB1-A68B-8D47F7AEBF4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA68A001-A2A5-49E6-A286-1CEA77E34894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="2" r:id="rId1"/>
@@ -23,10 +23,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -249,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -395,8 +395,19 @@
       <name val="Arial"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +508,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -651,8 +668,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1163,16 +1183,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1222,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1233,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1264,465 +1284,1378 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D336"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
         <v>101</v>
       </c>
-      <c r="C2" t="b">
+      <c r="C2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
         <v>102</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
         <v>103</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
         <v>104</v>
       </c>
-      <c r="C5" t="b">
+      <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
         <v>105</v>
       </c>
-      <c r="C6" t="b">
+      <c r="C6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <v>106</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
         <v>107</v>
       </c>
-      <c r="C8" t="b">
+      <c r="C8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>108</v>
       </c>
-      <c r="C9" t="b">
+      <c r="C9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10">
         <v>109</v>
       </c>
-      <c r="C10" t="b">
+      <c r="C10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>110</v>
       </c>
-      <c r="C11" t="b">
+      <c r="C11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>111</v>
       </c>
-      <c r="C12" t="b">
+      <c r="C12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>112</v>
       </c>
-      <c r="C13" t="b">
+      <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>113</v>
       </c>
-      <c r="C14" t="b">
+      <c r="C14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>114</v>
       </c>
-      <c r="C15" t="b">
+      <c r="C15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
         <v>115</v>
       </c>
-      <c r="C16" t="b">
+      <c r="C16" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
         <v>116</v>
       </c>
-      <c r="C17" t="b">
+      <c r="C17" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18">
         <v>117</v>
       </c>
-      <c r="C18" t="b">
+      <c r="C18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19">
         <v>118</v>
       </c>
-      <c r="C19" t="b">
+      <c r="C19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20">
         <v>119</v>
       </c>
-      <c r="C20" t="b">
+      <c r="C20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21">
         <v>120</v>
       </c>
-      <c r="C21" t="b">
+      <c r="C21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22">
         <v>121</v>
       </c>
-      <c r="C22" t="b">
+      <c r="C22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23">
         <v>122</v>
       </c>
-      <c r="C23" t="b">
+      <c r="C23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24">
         <v>123</v>
       </c>
-      <c r="C24" t="b">
+      <c r="C24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25">
         <v>124</v>
       </c>
-      <c r="C25" t="b">
+      <c r="C25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
       <c r="B26">
         <v>125</v>
       </c>
-      <c r="C26" t="b">
+      <c r="C26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27">
         <v>126</v>
       </c>
-      <c r="C27" t="b">
+      <c r="C27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28">
         <v>127</v>
       </c>
-      <c r="C28" t="b">
+      <c r="C28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
       <c r="B29">
         <v>128</v>
       </c>
-      <c r="C29" t="b">
+      <c r="C29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
       <c r="B30">
         <v>129</v>
       </c>
-      <c r="C30" t="b">
+      <c r="C30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
       <c r="B31">
         <v>130</v>
       </c>
-      <c r="C31" t="b">
+      <c r="C31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32">
         <v>131</v>
       </c>
-      <c r="C32" t="b">
+      <c r="C32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="1"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="1"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="1"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="1"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="1"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="1"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="1"/>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="1"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="1"/>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C189" s="1"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="1"/>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C191" s="1"/>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C192" s="1"/>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C193" s="1"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C194" s="1"/>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C195" s="1"/>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C196" s="1"/>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C197" s="1"/>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C198" s="1"/>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C199" s="1"/>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C200" s="1"/>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C201" s="1"/>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C202" s="1"/>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C203" s="1"/>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C204" s="1"/>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C205" s="1"/>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C206" s="1"/>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C207" s="1"/>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C208" s="1"/>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C209" s="1"/>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C210" s="1"/>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="1"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C212" s="1"/>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C213" s="1"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C214" s="1"/>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C215" s="1"/>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C216" s="1"/>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C217" s="1"/>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C218" s="1"/>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C219" s="1"/>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C220" s="1"/>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C221" s="1"/>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C222" s="1"/>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C223" s="1"/>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C224" s="1"/>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" s="1"/>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C226" s="1"/>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C227" s="1"/>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C228" s="1"/>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C229" s="1"/>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C230" s="1"/>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C231" s="1"/>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C232" s="1"/>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C233" s="1"/>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C234" s="1"/>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C235" s="1"/>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C236" s="1"/>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C237" s="1"/>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C238" s="1"/>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C239" s="1"/>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C240" s="1"/>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C241" s="1"/>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C242" s="1"/>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C243" s="1"/>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C244" s="1"/>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C245" s="1"/>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C246" s="1"/>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C247" s="1"/>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C248" s="1"/>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C249" s="1"/>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C250" s="1"/>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C251" s="1"/>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C252" s="1"/>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C253" s="1"/>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C254" s="1"/>
+    </row>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C255" s="1"/>
+    </row>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C256" s="1"/>
+    </row>
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C257" s="1"/>
+    </row>
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C258" s="1"/>
+    </row>
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C259" s="1"/>
+    </row>
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C260" s="1"/>
+    </row>
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C261" s="1"/>
+    </row>
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C262" s="1"/>
+    </row>
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C263" s="1"/>
+    </row>
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C264" s="1"/>
+    </row>
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C265" s="1"/>
+    </row>
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C266" s="1"/>
+    </row>
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C267" s="1"/>
+    </row>
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C268" s="1"/>
+    </row>
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C269" s="1"/>
+    </row>
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C270" s="1"/>
+    </row>
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C271" s="1"/>
+    </row>
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C272" s="1"/>
+    </row>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C273" s="1"/>
+    </row>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C274" s="1"/>
+    </row>
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C275" s="1"/>
+    </row>
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C276" s="1"/>
+    </row>
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C277" s="1"/>
+    </row>
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C278" s="1"/>
+    </row>
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C279" s="1"/>
+    </row>
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C280" s="1"/>
+    </row>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C281" s="1"/>
+    </row>
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C282" s="1"/>
+    </row>
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C283" s="1"/>
+    </row>
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C284" s="1"/>
+    </row>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C285" s="1"/>
+    </row>
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C286" s="1"/>
+    </row>
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C287" s="1"/>
+    </row>
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C288" s="1"/>
+    </row>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C289" s="1"/>
+    </row>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C290" s="1"/>
+    </row>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C291" s="1"/>
+    </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C292" s="1"/>
+    </row>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C293" s="1"/>
+    </row>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C294" s="1"/>
+    </row>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C295" s="1"/>
+    </row>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C296" s="1"/>
+    </row>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C297" s="1"/>
+    </row>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C298" s="1"/>
+    </row>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C299" s="1"/>
+    </row>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C300" s="1"/>
+    </row>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C301" s="1"/>
+    </row>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C302" s="1"/>
+    </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C303" s="1"/>
+    </row>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C304" s="1"/>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C305" s="1"/>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C306" s="1"/>
+    </row>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C307" s="1"/>
+    </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C308" s="1"/>
+    </row>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C309" s="1"/>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C310" s="1"/>
+    </row>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C311" s="1"/>
+    </row>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C312" s="2"/>
+    </row>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C313" s="2"/>
+    </row>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C314" s="2"/>
+    </row>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C315" s="2"/>
+    </row>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C316" s="2"/>
+    </row>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C317" s="2"/>
+    </row>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C318" s="2"/>
+    </row>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C319" s="2"/>
+    </row>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C320" s="2"/>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C321" s="2"/>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C322" s="2"/>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C323" s="2"/>
+    </row>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C324" s="2"/>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C325" s="2"/>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C326" s="2"/>
+    </row>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C327" s="2"/>
+    </row>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C328" s="2"/>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C329" s="2"/>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C330" s="2"/>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C331" s="2"/>
+    </row>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C332" s="2"/>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C333" s="2"/>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C334" s="2"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C335" s="2"/>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C336" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
fix outcome_ath 1_0 non_rep cohort_id
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\extender_outcomes_ath\20230321_outcomes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA68A001-A2A5-49E6-A286-1CEA77E34894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{CA68A001-A2A5-49E6-A286-1CEA77E34894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5478A64E-4D67-43A4-A819-27BED9F7C34D}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,10 +23,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -224,7 +224,7 @@
     <t xml:space="preserve">environage </t>
   </si>
   <si>
-    <t>no_name</t>
+    <t>helix</t>
   </si>
   <si>
     <t>pelagie</t>
@@ -239,17 +239,20 @@
     <t>hgs</t>
   </si>
   <si>
-    <t>recetox</t>
+    <t>elspac</t>
   </si>
   <si>
     <t>genxxi</t>
+  </si>
+  <si>
+    <t>genrnext</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -670,9 +673,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1187,12 +1190,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1287,17 +1290,17 @@
   <dimension ref="A1:D336"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C336"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1745,916 +1748,927 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>131</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3">
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3">
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3">
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3">
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3">
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3">
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3">
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3">
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3">
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3">
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3">
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3">
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3">
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3">
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3">
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3">
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3">
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3">
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3">
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3">
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3">
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3">
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3">
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3">
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3">
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3">
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3">
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3">
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3">
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3">
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3">
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3">
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3">
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3">
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3">
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3">
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3">
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3">
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3">
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3">
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3">
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3">
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3">
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3">
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3">
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3">
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3">
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3">
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3">
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3">
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3">
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3">
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3">
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3">
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3">
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3">
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3">
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3">
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3">
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3">
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3">
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3">
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3">
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3">
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3">
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3">
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3">
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3">
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3">
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3">
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3">
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3">
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3">
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3">
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3">
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3">
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3">
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3">
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3">
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3">
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3">
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3">
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3">
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3">
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3">
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3">
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3">
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3">
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3">
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3">
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3">
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3">
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3">
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3">
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3">
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3">
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3">
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3">
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3">
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3">
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3">
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3">
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3">
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3">
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3">
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3">
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3">
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3">
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3">
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3">
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3">
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3">
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3">
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3">
       <c r="C181" s="1"/>
     </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3">
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3">
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3">
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3">
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3">
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3">
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3">
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3">
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3">
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3">
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3">
       <c r="C192" s="1"/>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3">
       <c r="C193" s="1"/>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3">
       <c r="C194" s="1"/>
     </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3">
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3">
       <c r="C196" s="1"/>
     </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3">
       <c r="C197" s="1"/>
     </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3">
       <c r="C198" s="1"/>
     </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3">
       <c r="C199" s="1"/>
     </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3">
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3">
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3">
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3">
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3">
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3">
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3">
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3">
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3">
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3">
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3">
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3">
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3">
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3">
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3">
       <c r="C214" s="1"/>
     </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3">
       <c r="C215" s="1"/>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3">
       <c r="C216" s="1"/>
     </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3">
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3">
       <c r="C218" s="1"/>
     </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3">
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3">
       <c r="C220" s="1"/>
     </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3">
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3">
       <c r="C222" s="1"/>
     </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3">
       <c r="C223" s="1"/>
     </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3">
       <c r="C224" s="1"/>
     </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3">
       <c r="C225" s="1"/>
     </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3">
       <c r="C226" s="1"/>
     </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3">
       <c r="C227" s="1"/>
     </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3">
       <c r="C228" s="1"/>
     </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3">
       <c r="C229" s="1"/>
     </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3">
       <c r="C230" s="1"/>
     </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3">
       <c r="C231" s="1"/>
     </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3">
       <c r="C232" s="1"/>
     </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3">
       <c r="C233" s="1"/>
     </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3">
       <c r="C234" s="1"/>
     </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3">
       <c r="C235" s="1"/>
     </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3">
       <c r="C236" s="1"/>
     </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3">
       <c r="C237" s="1"/>
     </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3">
       <c r="C238" s="1"/>
     </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3">
       <c r="C239" s="1"/>
     </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3">
       <c r="C240" s="1"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3">
       <c r="C241" s="1"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3">
       <c r="C242" s="1"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3">
       <c r="C243" s="1"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3">
       <c r="C244" s="1"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3">
       <c r="C245" s="1"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3">
       <c r="C246" s="1"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3">
       <c r="C247" s="1"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3">
       <c r="C248" s="1"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3">
       <c r="C249" s="1"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3">
       <c r="C250" s="1"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3">
       <c r="C251" s="1"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3">
       <c r="C252" s="1"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3">
       <c r="C253" s="1"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3">
       <c r="C254" s="1"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3">
       <c r="C255" s="1"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3">
       <c r="C256" s="1"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3">
       <c r="C257" s="1"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3">
       <c r="C258" s="1"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3">
       <c r="C259" s="1"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3">
       <c r="C260" s="1"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3">
       <c r="C261" s="1"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3">
       <c r="C262" s="1"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3">
       <c r="C263" s="1"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3">
       <c r="C264" s="1"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3">
       <c r="C265" s="1"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3">
       <c r="C266" s="1"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3">
       <c r="C267" s="1"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3">
       <c r="C268" s="1"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3">
       <c r="C269" s="1"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3">
       <c r="C270" s="1"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3">
       <c r="C271" s="1"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3">
       <c r="C272" s="1"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3">
       <c r="C273" s="1"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3">
       <c r="C274" s="1"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3">
       <c r="C275" s="1"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3">
       <c r="C276" s="1"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3">
       <c r="C277" s="1"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3">
       <c r="C278" s="1"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3">
       <c r="C279" s="1"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3">
       <c r="C280" s="1"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3">
       <c r="C281" s="1"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3">
       <c r="C282" s="1"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3">
       <c r="C283" s="1"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3">
       <c r="C284" s="1"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3">
       <c r="C285" s="1"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3">
       <c r="C286" s="1"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3">
       <c r="C287" s="1"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3">
       <c r="C288" s="1"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3">
       <c r="C289" s="1"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3">
       <c r="C290" s="1"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3">
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3">
       <c r="C292" s="1"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3">
       <c r="C293" s="1"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3">
       <c r="C294" s="1"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3">
       <c r="C295" s="1"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3">
       <c r="C296" s="1"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3">
       <c r="C297" s="1"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3">
       <c r="C298" s="1"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3">
       <c r="C299" s="1"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3">
       <c r="C300" s="1"/>
     </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3">
       <c r="C301" s="1"/>
     </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3">
       <c r="C302" s="1"/>
     </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3">
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3">
       <c r="C304" s="1"/>
     </row>
-    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3">
       <c r="C305" s="1"/>
     </row>
-    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3">
       <c r="C306" s="1"/>
     </row>
-    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3">
       <c r="C307" s="1"/>
     </row>
-    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3">
       <c r="C308" s="1"/>
     </row>
-    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3">
       <c r="C309" s="1"/>
     </row>
-    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3">
       <c r="C310" s="1"/>
     </row>
-    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3">
       <c r="C311" s="1"/>
     </row>
-    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3">
       <c r="C312" s="2"/>
     </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3">
       <c r="C313" s="2"/>
     </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3">
       <c r="C314" s="2"/>
     </row>
-    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3">
       <c r="C315" s="2"/>
     </row>
-    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3">
       <c r="C316" s="2"/>
     </row>
-    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3">
       <c r="C317" s="2"/>
     </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3">
       <c r="C318" s="2"/>
     </row>
-    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3">
       <c r="C319" s="2"/>
     </row>
-    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3">
       <c r="C320" s="2"/>
     </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3">
       <c r="C321" s="2"/>
     </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3">
       <c r="C322" s="2"/>
     </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3">
       <c r="C323" s="2"/>
     </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3">
       <c r="C324" s="2"/>
     </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3">
       <c r="C325" s="2"/>
     </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3">
       <c r="C326" s="2"/>
     </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3">
       <c r="C327" s="2"/>
     </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3">
       <c r="C328" s="2"/>
     </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3">
       <c r="C329" s="2"/>
     </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3">
       <c r="C330" s="2"/>
     </row>
-    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3">
       <c r="C331" s="2"/>
     </row>
-    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3">
       <c r="C332" s="2"/>
     </row>
-    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3">
       <c r="C333" s="2"/>
     </row>
-    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3">
       <c r="C334" s="2"/>
     </row>
-    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3">
       <c r="C335" s="2"/>
     </row>
-    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3">
       <c r="C336" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor version bump Athlete outcome 1_1
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_non_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\extender_outcomes_ath\20230321_outcomes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{CA68A001-A2A5-49E6-A286-1CEA77E34894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02ABA8E4-FE23-461F-B333-774BFE2B453D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA68A001-A2A5-49E6-A286-1CEA77E34894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,10 +23,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -224,7 +224,7 @@
     <t xml:space="preserve">environage </t>
   </si>
   <si>
-    <t>helix</t>
+    <t>no_name</t>
   </si>
   <si>
     <t>pelagie</t>
@@ -239,20 +239,17 @@
     <t>hgs</t>
   </si>
   <si>
-    <t>elspac</t>
+    <t>recetox</t>
   </si>
   <si>
     <t>genxxi</t>
-  </si>
-  <si>
-    <t>genrnext</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -673,9 +670,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1190,12 +1187,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1245,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1290,17 +1287,17 @@
   <dimension ref="A1:D336"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C33" sqref="C33:C336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1314,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1328,7 +1325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1356,7 +1353,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1370,7 +1367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1384,7 +1381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1398,7 +1395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1412,7 +1409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1437,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1454,7 +1451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1468,7 +1465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1482,7 +1479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1496,7 +1493,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1510,7 +1507,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1608,7 +1605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1619,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1650,7 +1647,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1692,7 +1689,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1706,7 +1703,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1720,7 +1717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1734,7 +1731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1748,927 +1745,916 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33">
-        <v>132</v>
-      </c>
-      <c r="C33" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="3:3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="3:3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="3:3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="3:3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="3:3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="3:3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="3:3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="3:3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="3:3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="3:3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="3:3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="3:3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="3:3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="3:3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="3:3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="3:3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="3:3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="3:3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="3:3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="3:3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="3:3">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="3:3">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="3:3">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="3:3">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="3:3">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="3:3">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="3:3">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="3:3">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="3:3">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="3:3">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="3:3">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="3:3">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="3:3">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="3:3">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="3:3">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="3:3">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="3:3">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="3:3">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="3:3">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="3:3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="3:3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="3:3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="3:3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="3:3">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="3:3">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="3:3">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="3:3">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="3:3">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="3:3">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="3:3">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="3:3">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="3:3">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="3:3">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="3:3">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="3:3">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="3:3">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="3:3">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="3:3">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="3:3">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="3:3">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="3:3">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="3:3">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="3:3">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="3:3">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="3:3">
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="3:3">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="3:3">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="3:3">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="3:3">
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="3:3">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="3:3">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="3:3">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="3:3">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="3:3">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="3:3">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="3:3">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="3:3">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="3:3">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="3:3">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="3:3">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="3:3">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="3:3">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="3:3">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="3:3">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="3:3">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="3:3">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="3:3">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="3:3">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="3:3">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="3:3">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="3:3">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C181" s="1"/>
     </row>
-    <row r="182" spans="3:3">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="3:3">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="3:3">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="3:3">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="3:3">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="3:3">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="3:3">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="3:3">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="3:3">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="3:3">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="3:3">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C192" s="1"/>
     </row>
-    <row r="193" spans="3:3">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C193" s="1"/>
     </row>
-    <row r="194" spans="3:3">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C194" s="1"/>
     </row>
-    <row r="195" spans="3:3">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="3:3">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C196" s="1"/>
     </row>
-    <row r="197" spans="3:3">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C197" s="1"/>
     </row>
-    <row r="198" spans="3:3">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C198" s="1"/>
     </row>
-    <row r="199" spans="3:3">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C199" s="1"/>
     </row>
-    <row r="200" spans="3:3">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="3:3">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="3:3">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="3:3">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="3:3">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="3:3">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="3:3">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="3:3">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="3:3">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="3:3">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="3:3">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="3:3">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="3:3">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="3:3">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="3:3">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C214" s="1"/>
     </row>
-    <row r="215" spans="3:3">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C215" s="1"/>
     </row>
-    <row r="216" spans="3:3">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C216" s="1"/>
     </row>
-    <row r="217" spans="3:3">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="3:3">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C218" s="1"/>
     </row>
-    <row r="219" spans="3:3">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="3:3">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C220" s="1"/>
     </row>
-    <row r="221" spans="3:3">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="3:3">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C222" s="1"/>
     </row>
-    <row r="223" spans="3:3">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C223" s="1"/>
     </row>
-    <row r="224" spans="3:3">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C224" s="1"/>
     </row>
-    <row r="225" spans="3:3">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C225" s="1"/>
     </row>
-    <row r="226" spans="3:3">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C226" s="1"/>
     </row>
-    <row r="227" spans="3:3">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C227" s="1"/>
     </row>
-    <row r="228" spans="3:3">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C228" s="1"/>
     </row>
-    <row r="229" spans="3:3">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C229" s="1"/>
     </row>
-    <row r="230" spans="3:3">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C230" s="1"/>
     </row>
-    <row r="231" spans="3:3">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C231" s="1"/>
     </row>
-    <row r="232" spans="3:3">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C232" s="1"/>
     </row>
-    <row r="233" spans="3:3">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C233" s="1"/>
     </row>
-    <row r="234" spans="3:3">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C234" s="1"/>
     </row>
-    <row r="235" spans="3:3">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C235" s="1"/>
     </row>
-    <row r="236" spans="3:3">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C236" s="1"/>
     </row>
-    <row r="237" spans="3:3">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C237" s="1"/>
     </row>
-    <row r="238" spans="3:3">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C238" s="1"/>
     </row>
-    <row r="239" spans="3:3">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C239" s="1"/>
     </row>
-    <row r="240" spans="3:3">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C240" s="1"/>
     </row>
-    <row r="241" spans="3:3">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C241" s="1"/>
     </row>
-    <row r="242" spans="3:3">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C242" s="1"/>
     </row>
-    <row r="243" spans="3:3">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C243" s="1"/>
     </row>
-    <row r="244" spans="3:3">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C244" s="1"/>
     </row>
-    <row r="245" spans="3:3">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C245" s="1"/>
     </row>
-    <row r="246" spans="3:3">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C246" s="1"/>
     </row>
-    <row r="247" spans="3:3">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C247" s="1"/>
     </row>
-    <row r="248" spans="3:3">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C248" s="1"/>
     </row>
-    <row r="249" spans="3:3">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C249" s="1"/>
     </row>
-    <row r="250" spans="3:3">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C250" s="1"/>
     </row>
-    <row r="251" spans="3:3">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C251" s="1"/>
     </row>
-    <row r="252" spans="3:3">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C252" s="1"/>
     </row>
-    <row r="253" spans="3:3">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C253" s="1"/>
     </row>
-    <row r="254" spans="3:3">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C254" s="1"/>
     </row>
-    <row r="255" spans="3:3">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C255" s="1"/>
     </row>
-    <row r="256" spans="3:3">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C256" s="1"/>
     </row>
-    <row r="257" spans="3:3">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C257" s="1"/>
     </row>
-    <row r="258" spans="3:3">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C258" s="1"/>
     </row>
-    <row r="259" spans="3:3">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C259" s="1"/>
     </row>
-    <row r="260" spans="3:3">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C260" s="1"/>
     </row>
-    <row r="261" spans="3:3">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C261" s="1"/>
     </row>
-    <row r="262" spans="3:3">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C262" s="1"/>
     </row>
-    <row r="263" spans="3:3">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C263" s="1"/>
     </row>
-    <row r="264" spans="3:3">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C264" s="1"/>
     </row>
-    <row r="265" spans="3:3">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C265" s="1"/>
     </row>
-    <row r="266" spans="3:3">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C266" s="1"/>
     </row>
-    <row r="267" spans="3:3">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C267" s="1"/>
     </row>
-    <row r="268" spans="3:3">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C268" s="1"/>
     </row>
-    <row r="269" spans="3:3">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C269" s="1"/>
     </row>
-    <row r="270" spans="3:3">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C270" s="1"/>
     </row>
-    <row r="271" spans="3:3">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C271" s="1"/>
     </row>
-    <row r="272" spans="3:3">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C272" s="1"/>
     </row>
-    <row r="273" spans="3:3">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C273" s="1"/>
     </row>
-    <row r="274" spans="3:3">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C274" s="1"/>
     </row>
-    <row r="275" spans="3:3">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C275" s="1"/>
     </row>
-    <row r="276" spans="3:3">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C276" s="1"/>
     </row>
-    <row r="277" spans="3:3">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C277" s="1"/>
     </row>
-    <row r="278" spans="3:3">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C278" s="1"/>
     </row>
-    <row r="279" spans="3:3">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C279" s="1"/>
     </row>
-    <row r="280" spans="3:3">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C280" s="1"/>
     </row>
-    <row r="281" spans="3:3">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C281" s="1"/>
     </row>
-    <row r="282" spans="3:3">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C282" s="1"/>
     </row>
-    <row r="283" spans="3:3">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C283" s="1"/>
     </row>
-    <row r="284" spans="3:3">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C284" s="1"/>
     </row>
-    <row r="285" spans="3:3">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C285" s="1"/>
     </row>
-    <row r="286" spans="3:3">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C286" s="1"/>
     </row>
-    <row r="287" spans="3:3">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C287" s="1"/>
     </row>
-    <row r="288" spans="3:3">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C288" s="1"/>
     </row>
-    <row r="289" spans="3:3">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C289" s="1"/>
     </row>
-    <row r="290" spans="3:3">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C290" s="1"/>
     </row>
-    <row r="291" spans="3:3">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="3:3">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C292" s="1"/>
     </row>
-    <row r="293" spans="3:3">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C293" s="1"/>
     </row>
-    <row r="294" spans="3:3">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C294" s="1"/>
     </row>
-    <row r="295" spans="3:3">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C295" s="1"/>
     </row>
-    <row r="296" spans="3:3">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C296" s="1"/>
     </row>
-    <row r="297" spans="3:3">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C297" s="1"/>
     </row>
-    <row r="298" spans="3:3">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C298" s="1"/>
     </row>
-    <row r="299" spans="3:3">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C299" s="1"/>
     </row>
-    <row r="300" spans="3:3">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C300" s="1"/>
     </row>
-    <row r="301" spans="3:3">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C301" s="1"/>
     </row>
-    <row r="302" spans="3:3">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C302" s="1"/>
     </row>
-    <row r="303" spans="3:3">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="3:3">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C304" s="1"/>
     </row>
-    <row r="305" spans="3:3">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C305" s="1"/>
     </row>
-    <row r="306" spans="3:3">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C306" s="1"/>
     </row>
-    <row r="307" spans="3:3">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C307" s="1"/>
     </row>
-    <row r="308" spans="3:3">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C308" s="1"/>
     </row>
-    <row r="309" spans="3:3">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C309" s="1"/>
     </row>
-    <row r="310" spans="3:3">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C310" s="1"/>
     </row>
-    <row r="311" spans="3:3">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C311" s="1"/>
     </row>
-    <row r="312" spans="3:3">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C312" s="2"/>
     </row>
-    <row r="313" spans="3:3">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C313" s="2"/>
     </row>
-    <row r="314" spans="3:3">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C314" s="2"/>
     </row>
-    <row r="315" spans="3:3">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C315" s="2"/>
     </row>
-    <row r="316" spans="3:3">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C316" s="2"/>
     </row>
-    <row r="317" spans="3:3">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C317" s="2"/>
     </row>
-    <row r="318" spans="3:3">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C318" s="2"/>
     </row>
-    <row r="319" spans="3:3">
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C319" s="2"/>
     </row>
-    <row r="320" spans="3:3">
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C320" s="2"/>
     </row>
-    <row r="321" spans="3:3">
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321" s="2"/>
     </row>
-    <row r="322" spans="3:3">
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322" s="2"/>
     </row>
-    <row r="323" spans="3:3">
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323" s="2"/>
     </row>
-    <row r="324" spans="3:3">
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C324" s="2"/>
     </row>
-    <row r="325" spans="3:3">
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325" s="2"/>
     </row>
-    <row r="326" spans="3:3">
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C326" s="2"/>
     </row>
-    <row r="327" spans="3:3">
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C327" s="2"/>
     </row>
-    <row r="328" spans="3:3">
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C328" s="2"/>
     </row>
-    <row r="329" spans="3:3">
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329" s="2"/>
     </row>
-    <row r="330" spans="3:3">
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C330" s="2"/>
     </row>
-    <row r="331" spans="3:3">
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C331" s="2"/>
     </row>
-    <row r="332" spans="3:3">
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C332" s="2"/>
     </row>
-    <row r="333" spans="3:3">
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C333" s="2"/>
     </row>
-    <row r="334" spans="3:3">
+    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C334" s="2"/>
     </row>
-    <row r="335" spans="3:3">
+    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C335" s="2"/>
     </row>
-    <row r="336" spans="3:3">
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C336" s="2"/>
     </row>
   </sheetData>

</xml_diff>